<commit_message>
Graphical Notes Part I- Addeded
</commit_message>
<xml_diff>
--- a/Petros/Professional Work Process.xlsx
+++ b/Petros/Professional Work Process.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FAST BACKUP_DESKTOP\Career Related\Career Enhancement\Engineering Accelarator I\Fall 2017\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9100" yWindow="0" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="9105" yWindow="0" windowWidth="19440" windowHeight="12240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="1" r:id="rId1"/>
     <sheet name="Review Check List" sheetId="2" r:id="rId2"/>
     <sheet name="Release Checklist" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>Professional Work Process</t>
   </si>
@@ -108,13 +113,226 @@
   </si>
   <si>
     <t xml:space="preserve">Verision </t>
+  </si>
+  <si>
+    <t>Some times but not on regular bases</t>
+  </si>
+  <si>
+    <t>Working on Average around 10 hours</t>
+  </si>
+  <si>
+    <t>Best Coomunication method</t>
+  </si>
+  <si>
+    <t>Focuses on replying if late within 24 hours</t>
+  </si>
+  <si>
+    <t>Very good in communicating via e-mail</t>
+  </si>
+  <si>
+    <t>Used only on rare ocassions</t>
+  </si>
+  <si>
+    <t>It was not my prefered communication method</t>
+  </si>
+  <si>
+    <t>But over recent times, trying to use frequently</t>
+  </si>
+  <si>
+    <t>I use as safe and fast communication method in adition to e-mail</t>
+  </si>
+  <si>
+    <t>I use voice message incase of mising direct link</t>
+  </si>
+  <si>
+    <t>I usually return a call if late within 3 days since the missed call day</t>
+  </si>
+  <si>
+    <t>I use very rarely to this point</t>
+  </si>
+  <si>
+    <t>Only small conference videos</t>
+  </si>
+  <si>
+    <t>Always prefer phone unless some visual information is included</t>
+  </si>
+  <si>
+    <t>I specifically takes meeting minutes seriously</t>
+  </si>
+  <si>
+    <t>When leading meeting, I follow interactive meeting strategy</t>
+  </si>
+  <si>
+    <t>I share agenda atleast one week in advance unless it is confidential</t>
+  </si>
+  <si>
+    <t>When attending meeting, my startegy is focusing on listening and note taking</t>
+  </si>
+  <si>
+    <t>Keeping Questions only after the chance is given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usually recommends some pints at conclusion </t>
+  </si>
+  <si>
+    <t>Follow manager guidelines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report to maneger and suboardinates </t>
+  </si>
+  <si>
+    <t>Cross link with team members over a project</t>
+  </si>
+  <si>
+    <t>Mostly during emergency tight schedule</t>
+  </si>
+  <si>
+    <t>Prefer to carry on stages of the work process</t>
+  </si>
+  <si>
+    <t>Generation</t>
+  </si>
+  <si>
+    <t>Data collection and study</t>
+  </si>
+  <si>
+    <t>Reference to multiple sources and documenting as per the importance</t>
+  </si>
+  <si>
+    <t>Refining the sources and narrowing and redocumnting and clearing the less important information</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Mid work interruption for revising documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross checking the work done as of this stage </t>
+  </si>
+  <si>
+    <t>Keeping some notes of the finding and moving to the next procedures</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enumarating review criteria and enlisting according their importance level </t>
+  </si>
+  <si>
+    <t>Starting with the most detail review and documenting the finding</t>
+  </si>
+  <si>
+    <t>Documentation related to arvhive and documntation realted to managemnet reporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifically highlighting some severe issues finding and documenting in details </t>
+  </si>
+  <si>
+    <t>Preparing a written report on the finding of the review</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Documenting the final version of the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compiling all the documentation since the generation stage and archving </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Making a final comparision of the final version with the project definition </t>
+  </si>
+  <si>
+    <t>Basically depending on documentation minded</t>
+  </si>
+  <si>
+    <t>Focused on find and conquer strategy</t>
+  </si>
+  <si>
+    <t>Prefer to follow reporting based on severity</t>
+  </si>
+  <si>
+    <t>Error found</t>
+  </si>
+  <si>
+    <t>Stop the task</t>
+  </si>
+  <si>
+    <t>Find how severe the error is as per the project requiremnet</t>
+  </si>
+  <si>
+    <t>If severe report imediately and focus on some immediate remedies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If not that severe, </t>
+  </si>
+  <si>
+    <t>Take time to Enumerate solutions</t>
+  </si>
+  <si>
+    <t>If solution is found, exersise it and document the outtcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report also to superiors as per the project guidelines </t>
+  </si>
+  <si>
+    <t>Work closer with the managemnt to find fast solution</t>
+  </si>
+  <si>
+    <t>Implement any solution with the direct awareness of the manger</t>
+  </si>
+  <si>
+    <t>My strategy is focused on the following key techniques</t>
+  </si>
+  <si>
+    <t>We are all humans and we all make some mistakes in our life</t>
+  </si>
+  <si>
+    <t>As working colleagues the work is fisrt not idea dominance</t>
+  </si>
+  <si>
+    <t>Going deeper to the find the root cause of a problem occurrence</t>
+  </si>
+  <si>
+    <t>Listen to any idea before deciding on what to reply</t>
+  </si>
+  <si>
+    <t>This is at the bottom of my conflict rsolution strategies.</t>
+  </si>
+  <si>
+    <t>It works to start from oneself to identify the real cause of a conflict</t>
+  </si>
+  <si>
+    <t>And going down to every person involved to gather enough data</t>
+  </si>
+  <si>
+    <t>As working colleagues the work is first not an idea dominance</t>
+  </si>
+  <si>
+    <t>Putting a noble idea that all colleagues (invloved in conflict) work for succes of the project found at the center of solving many conflicts</t>
+  </si>
+  <si>
+    <t>Carrying extra investigation before acting on any conflict</t>
+  </si>
+  <si>
+    <t>Finding a wider and deper undertanding by taking some time</t>
+  </si>
+  <si>
+    <t>Collecting and documenting data related to conflicts</t>
+  </si>
+  <si>
+    <t>Countinoulsy listening to conflicting ideas and avoiding taking sides before replying</t>
+  </si>
+  <si>
+    <t>Petros Solomon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -151,14 +369,40 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -197,11 +441,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="25">
@@ -233,6 +484,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -558,47 +817,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="80" customWidth="1"/>
+    <col min="3" max="3" width="56.125" customWidth="1"/>
+    <col min="4" max="4" width="32.875" customWidth="1"/>
+    <col min="5" max="5" width="36.875" customWidth="1"/>
+    <col min="6" max="6" width="63.375" customWidth="1"/>
+    <col min="7" max="7" width="50.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -621,60 +883,313 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="D10" t="s">
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" t="s">
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="F13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="D14" t="s">
+      <c r="G13" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="5:6">
-      <c r="F18" t="s">
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="5:6">
+      <c r="G18" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="5:6">
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
       <c r="F22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="5:6">
-      <c r="F26" t="s">
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -688,40 +1203,40 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A21"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -745,37 +1260,37 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Work Process Comments Included and Updated
</commit_message>
<xml_diff>
--- a/Petros/Professional Work Process.xlsx
+++ b/Petros/Professional Work Process.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Review Check List" sheetId="2" r:id="rId2"/>
     <sheet name="Release Checklist" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,8 +25,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Petros Tsegay</author>
+  </authors>
+  <commentList>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Petros Tsegay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="112">
   <si>
     <t>Professional Work Process</t>
   </si>
@@ -310,9 +344,6 @@
     <t>As working colleagues the work is first not an idea dominance</t>
   </si>
   <si>
-    <t>Putting a noble idea that all colleagues (invloved in conflict) work for succes of the project found at the center of solving many conflicts</t>
-  </si>
-  <si>
     <t>Carrying extra investigation before acting on any conflict</t>
   </si>
   <si>
@@ -326,13 +357,52 @@
   </si>
   <si>
     <t>Petros Solomon</t>
+  </si>
+  <si>
+    <t>In normal situation works for  not more than 5 hours each day on average</t>
+  </si>
+  <si>
+    <t>Sometimes I go to work the whole night in addition to the day hours</t>
+  </si>
+  <si>
+    <t>More than 18 Hours</t>
+  </si>
+  <si>
+    <t>Design and document project implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report timely to mangemnet </t>
+  </si>
+  <si>
+    <t>Maintaining cohorent working procedures</t>
+  </si>
+  <si>
+    <t>Addreressing specific and urgent scinarios which could jeopardize the progress of a project</t>
+  </si>
+  <si>
+    <t>Analsying and giving some feedback on the project progress</t>
+  </si>
+  <si>
+    <t>Innition, planning and design of a project</t>
+  </si>
+  <si>
+    <t>Ooverseeing and monitoring project progress</t>
+  </si>
+  <si>
+    <t>Supporting in times of need and when there is a difficulty facing in pushing the progress of the project before deadline</t>
+  </si>
+  <si>
+    <t>Attending meeting and commenting positively on over all project progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Putting a noble idea that all colleagues (invloved in conflict) work for succes of the project </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -365,21 +435,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,29 +486,173 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -441,19 +683,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -816,392 +1080,576 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="19" zoomScaleNormal="19" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.875" customWidth="1"/>
-    <col min="2" max="2" width="80" customWidth="1"/>
+    <col min="2" max="2" width="82.25" customWidth="1"/>
     <col min="3" max="3" width="56.125" customWidth="1"/>
-    <col min="4" max="4" width="32.875" customWidth="1"/>
-    <col min="5" max="5" width="36.875" customWidth="1"/>
-    <col min="6" max="6" width="63.375" customWidth="1"/>
-    <col min="7" max="7" width="50.5" customWidth="1"/>
+    <col min="4" max="4" width="64.125" customWidth="1"/>
+    <col min="5" max="5" width="99.5" customWidth="1"/>
+    <col min="6" max="6" width="67.25" customWidth="1"/>
+    <col min="7" max="7" width="79.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="29" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="H7" s="23"/>
+      <c r="I7" s="21"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F8" t="s">
+      <c r="D8" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F9" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="21" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="4" t="s">
+      <c r="H9" s="23"/>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="21" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="H10" s="23"/>
+      <c r="I10" s="21"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="21" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="H11" s="23"/>
+      <c r="I11" s="21"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="21"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" s="18"/>
+      <c r="E13" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="H13" s="23"/>
+      <c r="I13" s="21"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="10" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="H14" s="23"/>
+      <c r="I14" s="21"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="10" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="H15" s="23"/>
+      <c r="I15" s="21"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="H16" s="23"/>
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="D17" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="D18" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="H18" s="23"/>
+      <c r="I18" s="21"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E19" t="s">
+      <c r="D19" s="18"/>
+      <c r="E19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="21"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="21"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="21"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="H22" s="23"/>
+      <c r="I22" s="21"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" s="23"/>
+      <c r="I23" s="21"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H24" s="23"/>
+      <c r="I24" s="21"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="21"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="23"/>
+      <c r="I26" s="21"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="H27" s="23"/>
+      <c r="I27" s="21"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F28" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+      <c r="G28" s="5"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="21"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+      <c r="G29" s="5"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="21"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
+      <c r="G30" s="5"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="21"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
+      <c r="G31" s="5"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="21"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="7" t="s">
         <v>48</v>
       </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="21"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>